<commit_message>
alteracao diagramas de atualizar stock
</commit_message>
<xml_diff>
--- a/Use Cases - Gestão de fábrica.xlsx
+++ b/Use Cases - Gestão de fábrica.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Documents\MIEI\3º Ano\1º Semestre\Desenvolvimento de Sistemas de Software\Projeto\dss-projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedroferreira/Desktop/DSS/dss-projeto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456EFF5F-A508-4CFD-8C86-F32AC9A4FFFA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="16005" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Registar Entrada Stock" sheetId="2" r:id="rId1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
   <si>
     <t xml:space="preserve">1.1. Regista componente no sistema </t>
   </si>
@@ -84,47 +83,10 @@
     <t>Use Case:</t>
   </si>
   <si>
-    <t>2.3.2. Informa que seleção foi cancelada</t>
-  </si>
-  <si>
-    <t>2.3.1. Não aceita registar componente</t>
-  </si>
-  <si>
-    <t>Cenário Exceção 3
-[não aceitar registar componente]
-(passo 2.3)</t>
-  </si>
-  <si>
     <t>4.2. Informa que seleção foi cancelada</t>
   </si>
   <si>
     <t>4.1. Não indica a quantidade</t>
-  </si>
-  <si>
-    <t>Cenário Exceção 2
-[não indica quantidades]
-(passo 4)</t>
-  </si>
-  <si>
-    <t>2.5. Regressa a 3</t>
-  </si>
-  <si>
-    <t>2.4. Regista componente no sistema</t>
-  </si>
-  <si>
-    <t>2.3. Aceita registar componente</t>
-  </si>
-  <si>
-    <t>2.2. Pergunta se quer adicionar componente ao sistema</t>
-  </si>
-  <si>
-    <t>2.1. Indica que componente não existe
- no sistema</t>
-  </si>
-  <si>
-    <t>Cenário Alternativo 1
-[componente não existe no sistema]
-(passo 2)</t>
   </si>
   <si>
     <t>2.2. Informa que seleção foi cancelada</t>
@@ -138,28 +100,16 @@
 (passo 2)</t>
   </si>
   <si>
-    <t>5. Encomenda o componente indicado</t>
-  </si>
-  <si>
     <t>4. Indica a quantidade</t>
   </si>
   <si>
-    <t>3. Pergunta qual a quantidade a encomendar</t>
-  </si>
-  <si>
     <t>2. Indica componente</t>
   </si>
   <si>
     <t>1. Apresenta lista de stock</t>
   </si>
   <si>
-    <t>Componente encomendado</t>
-  </si>
-  <si>
     <t>Funcionário autenticado</t>
-  </si>
-  <si>
-    <t>Encomendar Stock</t>
   </si>
   <si>
     <t>2.2. Informa que o procedimento 
@@ -258,11 +208,76 @@
   <si>
     <t>1.3. Regressa a 2</t>
   </si>
+  <si>
+    <t>Registar Stock</t>
+  </si>
+  <si>
+    <t>Stock do componente incrementado</t>
+  </si>
+  <si>
+    <t>3. Pergunta qual a quantidade a registar</t>
+  </si>
+  <si>
+    <t>5. Incrementa stock na quantidade indicada</t>
+  </si>
+  <si>
+    <t>Cenário Alternativo 1
+[componente não existe no sistema]
+(passo 3)</t>
+  </si>
+  <si>
+    <t>3.1. Indica que componente não existe
+ no sistema</t>
+  </si>
+  <si>
+    <t>3.2. Pergunta se quer adicionar componente ao sistema</t>
+  </si>
+  <si>
+    <t>3.3. Aceita registar componente</t>
+  </si>
+  <si>
+    <t>3.4 Pede para inserir dados do componente</t>
+  </si>
+  <si>
+    <t>3.5. Indica dados do componente</t>
+  </si>
+  <si>
+    <t>3.6. Regista componente no sistema</t>
+  </si>
+  <si>
+    <t>3.7. Regressa a 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cenário Exceção 3
+[existem dados por indicar]
+(passo 3.6)
+</t>
+  </si>
+  <si>
+    <t>3.6.1 Informa que seleção foi cancelada</t>
+  </si>
+  <si>
+    <t>3.3.2. Informa que seleção foi cancelada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cenário Exceção 2
+[não aceitar registar componente]
+(passo 3.3)
+</t>
+  </si>
+  <si>
+    <t>Cenário Exceção 4
+[não indica quantidades]
+(passo 4)</t>
+  </si>
+  <si>
+    <t>3.3.1 Indica que não quer registar componente</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -299,7 +314,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -442,11 +457,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -483,7 +550,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -512,6 +578,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -536,19 +608,23 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -829,18 +905,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D13"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.375" customWidth="1"/>
-    <col min="3" max="3" width="36.625" customWidth="1"/>
-    <col min="4" max="4" width="40.625" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" customWidth="1"/>
+    <col min="4" max="4" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -848,40 +924,40 @@
       <c r="B2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="32"/>
-    </row>
-    <row r="3" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D2" s="33"/>
+    </row>
+    <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="32"/>
-    </row>
-    <row r="4" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D3" s="33"/>
+    </row>
+    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="34"/>
-    </row>
-    <row r="5" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D4" s="35"/>
+    </row>
+    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="32"/>
-    </row>
-    <row r="6" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="29" t="s">
+      <c r="D5" s="33"/>
+    </row>
+    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="30" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="14" t="s">
@@ -891,34 +967,34 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="30"/>
+    <row r="7" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="31"/>
       <c r="C7" s="12" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="11"/>
     </row>
-    <row r="8" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="30"/>
+    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="31"/>
       <c r="C8" s="12" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="30"/>
+    <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="31"/>
       <c r="C9" s="12"/>
       <c r="D9" s="11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="30"/>
+    <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="31"/>
       <c r="C10" s="10"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="2:4" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="29" t="s">
+    <row r="11" spans="2:4" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="30" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -926,18 +1002,18 @@
       </c>
       <c r="D11" s="9"/>
     </row>
-    <row r="12" spans="2:4" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="30"/>
+    <row r="12" spans="2:4" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="31"/>
       <c r="C12" s="3"/>
       <c r="D12" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="30"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="31"/>
       <c r="C13" s="7"/>
       <c r="D13" s="6" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -955,18 +1031,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:D23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:D25"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.375" customWidth="1"/>
-    <col min="3" max="3" width="36.625" customWidth="1"/>
-    <col min="4" max="4" width="46.125" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" customWidth="1"/>
+    <col min="4" max="4" width="46.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -974,40 +1050,40 @@
       <c r="B2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="32"/>
-    </row>
-    <row r="3" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="33"/>
+    </row>
+    <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="32"/>
-    </row>
-    <row r="4" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D3" s="33"/>
+    </row>
+    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="32"/>
-    </row>
-    <row r="5" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="33"/>
+    </row>
+    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="32"/>
-    </row>
-    <row r="6" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="29" t="s">
+      <c r="C5" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="33"/>
+    </row>
+    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="30" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="14" t="s">
@@ -1017,134 +1093,154 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="29"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="30"/>
+    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="30"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="31"/>
       <c r="C8" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="22"/>
-    </row>
-    <row r="9" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="30"/>
+        <v>22</v>
+      </c>
+      <c r="D8" s="21"/>
+    </row>
+    <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="31"/>
       <c r="C9" s="12"/>
-      <c r="D9" s="22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="30"/>
+      <c r="D9" s="21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="31"/>
       <c r="C10" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="22"/>
-    </row>
-    <row r="11" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="30"/>
+        <v>21</v>
+      </c>
+      <c r="D10" s="21"/>
+    </row>
+    <row r="11" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="31"/>
       <c r="C11" s="10"/>
       <c r="D11" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>29</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>19</v>
       </c>
       <c r="D12" s="9"/>
     </row>
-    <row r="13" spans="2:4" ht="85.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="36"/>
+    <row r="13" spans="2:4" ht="85.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="37"/>
       <c r="C13" s="10"/>
-      <c r="D13" s="20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="35"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="42" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="35"/>
-      <c r="C16" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="35"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D13" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="36"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="36"/>
+      <c r="C16" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="29"/>
+    </row>
+    <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="36"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="36"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="9"/>
-    </row>
-    <row r="20" spans="2:4" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="36"/>
+      <c r="C18" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="36"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="37"/>
       <c r="C20" s="7"/>
-      <c r="D20" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="17" t="s">
+      <c r="D20" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="38" x14ac:dyDescent="0.25">
+      <c r="B21" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="43"/>
+    </row>
+    <row r="22" spans="2:4" ht="80" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="40"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="42" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="134" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="10"/>
+      <c r="D23" s="19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="38"/>
-    </row>
-    <row r="22" spans="2:4" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="39"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="41" t="s">
+      <c r="D24" s="9"/>
+    </row>
+    <row r="25" spans="2:4" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="37"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D23" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="B14:B18"/>
     <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B14:B20"/>
+    <mergeCell ref="B24:B25"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
@@ -1158,17 +1254,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:D16"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23.375" customWidth="1"/>
-    <col min="3" max="3" width="27.625" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
     <col min="4" max="4" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1177,40 +1273,40 @@
       <c r="B5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="32"/>
-    </row>
-    <row r="6" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="33"/>
+    </row>
+    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="32"/>
-    </row>
-    <row r="7" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="33"/>
+    </row>
+    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="32"/>
-    </row>
-    <row r="8" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="33"/>
+    </row>
+    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="32"/>
-    </row>
-    <row r="9" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="29" t="s">
+      <c r="C8" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="33"/>
+    </row>
+    <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="30" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="14" t="s">
@@ -1220,52 +1316,52 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="30"/>
+    <row r="10" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="31"/>
       <c r="C10" s="10"/>
       <c r="D10" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="30"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="31"/>
       <c r="C11" s="12" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D11" s="11"/>
     </row>
-    <row r="12" spans="2:4" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="30"/>
+    <row r="12" spans="2:4" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="31"/>
       <c r="C12" s="10"/>
-      <c r="D12" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="30"/>
+      <c r="D12" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="31"/>
       <c r="C13" s="10"/>
       <c r="D13" s="11"/>
     </row>
-    <row r="14" spans="2:4" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="26" t="s">
-        <v>40</v>
+    <row r="14" spans="2:4" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>26</v>
       </c>
       <c r="D14" s="9"/>
     </row>
-    <row r="15" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="30"/>
+    <row r="15" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="31"/>
       <c r="C15" s="10"/>
       <c r="D15" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="26.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="30"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="26" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="31"/>
       <c r="C16" s="7"/>
-      <c r="D16" s="25"/>
+      <c r="D16" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1282,18 +1378,18 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.625" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
-    <col min="4" max="4" width="40.625" customWidth="1"/>
+    <col min="4" max="4" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1301,40 +1397,40 @@
       <c r="B4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="32"/>
-    </row>
-    <row r="5" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="33"/>
+    </row>
+    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="32"/>
-    </row>
-    <row r="6" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D5" s="33"/>
+    </row>
+    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="32"/>
-    </row>
-    <row r="7" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="33"/>
+    </row>
+    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="32"/>
-    </row>
-    <row r="8" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="29" t="s">
+      <c r="C7" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="33"/>
+    </row>
+    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="30" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="14" t="s">
@@ -1344,96 +1440,96 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="30"/>
+    <row r="9" spans="2:4" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="31"/>
       <c r="C9" s="10"/>
-      <c r="D9" s="20" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="30"/>
+      <c r="D9" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="31"/>
       <c r="C10" s="12" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D10" s="11"/>
     </row>
-    <row r="11" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="30"/>
+    <row r="11" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="31"/>
       <c r="C11" s="10"/>
       <c r="D11" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="30"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="31"/>
       <c r="C12" s="10"/>
       <c r="D12" s="11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="30"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="31"/>
       <c r="C13" s="10"/>
       <c r="D13" s="11"/>
     </row>
-    <row r="14" spans="2:4" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="28"/>
+    <row r="14" spans="2:4" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="27"/>
       <c r="D14" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="35"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="36"/>
       <c r="C15" s="10"/>
       <c r="D15" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="35"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="36"/>
       <c r="C16" s="12" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="35"/>
+    <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="36"/>
       <c r="C17" s="10"/>
       <c r="D17" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="36"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="37"/>
       <c r="C18" s="10"/>
       <c r="D18" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="21"/>
-    </row>
-    <row r="20" spans="2:4" ht="80.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="35"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="20"/>
+    </row>
+    <row r="20" spans="2:4" ht="80.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="36"/>
       <c r="C20" s="7"/>
       <c r="D20" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
acho que nao tinha gravado...
</commit_message>
<xml_diff>
--- a/Use Cases - Gestão de fábrica.xlsx
+++ b/Use Cases - Gestão de fábrica.xlsx
@@ -9,13 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19860" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Registar Entrada Stock" sheetId="2" r:id="rId1"/>
-    <sheet name="Encomendar Stock" sheetId="3" r:id="rId2"/>
-    <sheet name="Consultar encomenda" sheetId="4" r:id="rId3"/>
-    <sheet name="Processar Encomenda" sheetId="5" r:id="rId4"/>
+    <sheet name="Encomendar Stock" sheetId="3" r:id="rId1"/>
+    <sheet name="Consultar encomenda" sheetId="4" r:id="rId2"/>
+    <sheet name="Produzir Encomenda" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -30,24 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
-  <si>
-    <t xml:space="preserve">1.1. Regista componente no sistema </t>
-  </si>
-  <si>
-    <t>Cenário Alternativo 1
-[componente não listada]
-(passo 1)</t>
-  </si>
-  <si>
-    <t>3. Atualiza o stock atual</t>
-  </si>
-  <si>
-    <t>2. Indica stock do componente</t>
-  </si>
-  <si>
-    <t>1. Seleciona o componente a atualizar o stock</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="60">
   <si>
     <t>System response</t>
   </si>
@@ -59,15 +41,9 @@
 Normal</t>
   </si>
   <si>
-    <t>Stock da componente é atualizado</t>
-  </si>
-  <si>
     <t>Pós condição:</t>
   </si>
   <si>
-    <t>Chegada de stock</t>
-  </si>
-  <si>
     <t>Pré condição:</t>
   </si>
   <si>
@@ -75,9 +51,6 @@
   </si>
   <si>
     <t>Actor:</t>
-  </si>
-  <si>
-    <t>Registar stock de componente</t>
   </si>
   <si>
     <t>Use Case:</t>
@@ -200,15 +173,6 @@
     <t>Encomenda processada</t>
   </si>
   <si>
-    <t>Processar Encomenda</t>
-  </si>
-  <si>
-    <t>1.2. Adiciona componente ao sistema</t>
-  </si>
-  <si>
-    <t>1.3. Regressa a 2</t>
-  </si>
-  <si>
     <t>Registar Stock</t>
   </si>
   <si>
@@ -272,6 +236,9 @@
   </si>
   <si>
     <t>3.3.1 Indica que não quer registar componente</t>
+  </si>
+  <si>
+    <t>Produzir Encomenda</t>
   </si>
 </sst>
 </file>
@@ -513,7 +480,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -521,13 +488,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -584,6 +545,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -599,32 +572,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -906,136 +864,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D13"/>
-  <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" customWidth="1"/>
-    <col min="4" max="4" width="40.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="33"/>
-    </row>
-    <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="33"/>
-    </row>
-    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="35"/>
-    </row>
-    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="33"/>
-    </row>
-    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="31"/>
-      <c r="C7" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="11"/>
-    </row>
-    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="31"/>
-      <c r="C8" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="11"/>
-    </row>
-    <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="31"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="31"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="2:4" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="9"/>
-    </row>
-    <row r="12" spans="2:4" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="31"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="31"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B10"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1047,193 +879,193 @@
   <sheetData>
     <row r="1" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="35"/>
+    </row>
+    <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="35"/>
+    </row>
+    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="35"/>
+    </row>
+    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="35"/>
+    </row>
+    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="32"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="32" t="s">
+    </row>
+    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="33"/>
+      <c r="C8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="19"/>
+    </row>
+    <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="33"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="33"/>
+      <c r="C10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="19"/>
+    </row>
+    <row r="11" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="33"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="2:4" ht="85.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="40"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="39"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="39"/>
+      <c r="C16" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="27"/>
+    </row>
+    <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="39"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="39"/>
+      <c r="C18" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="39"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="40"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="33"/>
-    </row>
-    <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="33"/>
-    </row>
-    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="33"/>
-    </row>
-    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="15" t="s">
+    </row>
+    <row r="21" spans="2:4" ht="38" x14ac:dyDescent="0.25">
+      <c r="B21" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="31"/>
+    </row>
+    <row r="22" spans="2:4" ht="80" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="38"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="134" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="33"/>
-    </row>
-    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="30"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="31"/>
-      <c r="C8" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="21"/>
-    </row>
-    <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="31"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="21" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="31"/>
-      <c r="C10" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="21"/>
-    </row>
-    <row r="11" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="31"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="9"/>
-    </row>
-    <row r="13" spans="2:4" ht="85.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="37"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="36"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="29" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="36"/>
-      <c r="C16" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="29"/>
-    </row>
-    <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="36"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="29" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="36"/>
-      <c r="C18" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="36"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="37"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="38" x14ac:dyDescent="0.25">
-      <c r="B21" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="41" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" s="43"/>
-    </row>
-    <row r="22" spans="2:4" ht="80" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="40"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="42" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="134" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" s="9"/>
+      <c r="D24" s="7"/>
     </row>
     <row r="25" spans="2:4" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="37"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="6" t="s">
-        <v>16</v>
+      <c r="B25" s="40"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1253,12 +1085,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:D16"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1270,98 +1102,98 @@
   <sheetData>
     <row r="4" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="33"/>
+      <c r="B5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="35"/>
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="33"/>
+      <c r="B6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="35"/>
     </row>
     <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="33"/>
+      <c r="B7" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="35"/>
     </row>
     <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="33"/>
+      <c r="B8" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="35"/>
     </row>
     <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>5</v>
+      <c r="B9" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="31"/>
-      <c r="C10" s="10"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="8"/>
       <c r="D10" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="31"/>
-      <c r="C11" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="11"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="9"/>
     </row>
     <row r="12" spans="2:4" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="31"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="19" t="s">
-        <v>28</v>
+      <c r="B12" s="33"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="17" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="31"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="11"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="2:4" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="9"/>
+      <c r="B14" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="7"/>
     </row>
     <row r="15" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="31"/>
-      <c r="C15" s="10"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="8"/>
       <c r="D15" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="26" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="31"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="24"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1377,12 +1209,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D21"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1394,142 +1226,142 @@
   <sheetData>
     <row r="3" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="33"/>
+      <c r="B4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="35"/>
     </row>
     <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="33"/>
+      <c r="B5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="35"/>
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="32" t="s">
+      <c r="B6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="35"/>
+    </row>
+    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="35"/>
+    </row>
+    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="33"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="33"/>
+      <c r="C10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="33"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="33"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="33"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="2:4" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="25"/>
+      <c r="D14" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="39"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="39"/>
+      <c r="C16" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="33"/>
-    </row>
-    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="33"/>
-    </row>
-    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="31"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="31"/>
-      <c r="C10" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="11"/>
-    </row>
-    <row r="11" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="31"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="31"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="31"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="11"/>
-    </row>
-    <row r="14" spans="2:4" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="36"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="36"/>
-      <c r="C16" s="12" t="s">
-        <v>40</v>
-      </c>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="36"/>
-      <c r="C17" s="10"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="8"/>
       <c r="D17" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="37"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="8" t="s">
-        <v>38</v>
+      <c r="B18" s="40"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="20"/>
+      <c r="B19" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="18"/>
     </row>
     <row r="20" spans="2:4" ht="80.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="36"/>
-      <c r="C20" s="7"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="5"/>
       <c r="D20" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>